<commit_message>
Modified the System Level Test spreadsheet, has about 40 steps with specific detail, writing it made me realize just how bad this program really is. I thought of how things should flow logically, and time after time, they did not in the program.
</commit_message>
<xml_diff>
--- a/System Level Tests/System Level Test Sheet.xlsx
+++ b/System Level Tests/System Level Test Sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>Name of Tester</t>
   </si>
@@ -68,35 +68,385 @@
     <t>Launch the program</t>
   </si>
   <si>
-    <t>Program starts, displays introduction</t>
-  </si>
-  <si>
     <t>Enter name</t>
   </si>
   <si>
-    <t>Name is entered, saved into object (doesn't break on odd characters) and displayed</t>
-  </si>
-  <si>
-    <t>Continue to game</t>
-  </si>
-  <si>
-    <t>Display Main Menu</t>
-  </si>
-  <si>
-    <t>Navigate through menu items</t>
-  </si>
-  <si>
-    <t>Display menus, find menus that are incomplete or not working</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etc… </t>
+    <t>Press Any Key</t>
+  </si>
+  <si>
+    <t>Press N or n</t>
+  </si>
+  <si>
+    <t>A new game is started. The main game object is created, several different variables like locations are initialized, random objects are placed in the several areas, and the player object is assigned to the start location. The Game Menu is then displayed. ****************************************
+                 Game Menu              
+D : Display Map
+M : Move player
+LI: Look around for items
+LP: Display People at this location
+S : Display scene list
+F : Finish Game
+I : Player Inventory
+P : Print Player Inventory Report to Disk
+PI : Print Location Inventory Report to Disk
+Q : Quit
+****************************************</t>
+  </si>
+  <si>
+    <t>Press D or d to display Map</t>
+  </si>
+  <si>
+    <t>Map is displayed
+   |   1  |   2  |   3  |   4  |   5  |
+1 |  HB  |* ST *|  AP  |  BU  |  CA  |
+2 |  DS  |  UD  |  FS  |  GS  |  HW  |
+3 |  FS  |  JY  |  CS  |  LI  |  MA  |
+4 |  GS  |  PO  |  PS  |  RE  |  AR  |
+5 |  ES  |  TH  |  UN  |  JJ  |  CH  |
+Press any key to continue...</t>
+  </si>
+  <si>
+    <t>Press any key</t>
+  </si>
+  <si>
+    <t>Game menu is displayed again
+****************************************
+                 Game Menu              
+D : Display Map
+M : Move player
+LI: Look around for items
+LP: Display People at this location
+S : Display scene list
+F : Finish Game
+I : Player Inventory
+P : Print Player Inventory Report to Disk
+PI : Print Location Inventory Report to Disk
+Q : Quit
+****************************************</t>
+  </si>
+  <si>
+    <t>Try input that isn't part of the menu: !</t>
+  </si>
+  <si>
+    <t>Prints "Invalid selection. Try again." Main menu is displayed again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type m or M </t>
+  </si>
+  <si>
+    <t>Displays the Move Player menu
+****************************************
+                  Move Player Menu              
+ Choose a location to travel to with letters:        
+ U : Up
+ Do : Down
+ L : Left
+ R : Right
+ Choose a location to travel to with WASD:        
+ W : Up
+ S : Down
+ A : Left
+ D : Right
+ Choose a location to travel to with 10-key numbers:        
+ 8 : Up
+ 5 : Down
+ 4 : Left
+ 6 : Right
+Q : Quit Previous Menu
+****************************************</t>
+  </si>
+  <si>
+    <t>Try each of the movement inputs</t>
+  </si>
+  <si>
+    <t>If the direction selected is invalid, display an error "You can't move that way" and then display the map, then print the move menu again. If a valid direction is selected, the player's location is updated, the map is displayed, and then the move menu is displayed again.</t>
+  </si>
+  <si>
+    <t>Press q on the movement menu to return to the main menu</t>
+  </si>
+  <si>
+    <t>Main menu is displayed.</t>
+  </si>
+  <si>
+    <t>Type LI or li</t>
+  </si>
+  <si>
+    <t>Area inventory is displayed (essentially, items on the ground)
+****************************************
+                 Inventory              
+  Name and Cost                         
+1. Name:Resource     Cost: 200
+2. Name:Shotgun     Cost: 10
+Q : Quit Inventory
+****************************************</t>
+  </si>
+  <si>
+    <t>Try typing 1 or 2 to inspect the items</t>
+  </si>
+  <si>
+    <t>Displays the item stats screen
+****************************************
+                Item Stats              
+Item Name: Resource
+Item Cost: 200
+Item Type: 0
+ D : Drop Item
+ P : Add item to player inventory
+ Q : Go Back to Inventory
+****************************************</t>
+  </si>
+  <si>
+    <t>Press p to pick up the item</t>
+  </si>
+  <si>
+    <t>Item is removed from area inventory, and added to player inventory, player is returned to the area inventory screen, which displays the inventory sans the item that was picked up</t>
+  </si>
+  <si>
+    <t>Note: my program actually fails this test. We didn't finish polishing this program, so there are many bugs in it. In this case, the player needs to hit q to return to inventory after picking up the item, and the area inventory is not updated to reflect the removal of the item until the LI menu item from the Game Menu is called again.</t>
+  </si>
+  <si>
+    <t>Press q to return to the Game Menu</t>
+  </si>
+  <si>
+    <t>The Game Menu is properly displayed again.</t>
+  </si>
+  <si>
+    <t>Type LP to look for people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Displays a menu similar to the Item Menu, but with the characters in the area. </t>
+  </si>
+  <si>
+    <t>Note: this was never implemented. Right now it returns null</t>
+  </si>
+  <si>
+    <t>Displays a character's back story. Displays the character menu, and the player may invite the character to join the party</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Name is entered.  Main player object is initialized, and the name is added to it. Displays the confirmation screen: 
+****************************************
+ Welcome to the game, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ You will probably die. Our condolences.
+****************************************
+Press any key to continue...</t>
+    </r>
+  </si>
+  <si>
+    <t>Main Menu is displayed. 
+****************************************
+                 Main Menu              
+N : Start a new game
+L : Load a saved game
+S : Save the game
+H : Get help, because you are a noob
+G : Game Menu
+Q : Quit
+****************************************</t>
+  </si>
+  <si>
+    <t>Press the appropriate number to talk to a character in the area</t>
+  </si>
+  <si>
+    <t>Press I to invite the character to join the party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The character's id is removed from the default area party and added to the player's party. Character now moves with the player from area to area. </t>
+  </si>
+  <si>
+    <t>Game menu is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program starts, displays introduction text 
+****************************************
+ This is the game of Zombie Oregon Trail
+ In this game you will help yourself try
+ to survive traveling to a safe ne place
+ while surviving zombies
+ To survive this trip you will need to
+ gather resources to like food, weapons,
+ wather, and shelter. You are not alone
+ however and may encounter new friends
+ and foes. Once you have enough resources
+ head to home base, pack your stuff and go
+ Do you have what it takes? or will you be
+ another meal for the undead?
+Please enter your name: </t>
+  </si>
+  <si>
+    <t>Type S to display the scene list</t>
+  </si>
+  <si>
+    <t>The list of scenes are displayed. It was a requirement for the program that there be a certain number of scenes for the text-based game, and that a method be created to display them. This prints all of the text out for the different scenes and then promptly displays the main menu again.</t>
+  </si>
+  <si>
+    <t>Type F to finish the game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I hated having this option here, but one of the other team-mates did it. </t>
+  </si>
+  <si>
+    <t>Typing F will check if the player has collected enough resources to escape the Zombie City, and either display a Congratulatory message that the player has won the game, and exit to the Main Menu, or display an error that the player lacks resources and cannot leave yet, then displays the Game Menu again.</t>
+  </si>
+  <si>
+    <t>Type I to display the player inventory</t>
+  </si>
+  <si>
+    <t>Displays the inventory screen. Each item that is contained in the ArrayList of the Player's inventory is printed to the screen. Like the ground inventory, each item can be inspected by typeing the appropriate number. The item can also be dropped from the inspection menu, and the item object will be transferred from the player inventory array to the area inventory array.</t>
+  </si>
+  <si>
+    <t>Press any appropriate number key to inspect an item</t>
+  </si>
+  <si>
+    <t>Display the item menu, display options to return to inventory (q) or drop the item on the ground (d)</t>
+  </si>
+  <si>
+    <t>Type d to drop an item to the groun</t>
+  </si>
+  <si>
+    <t>The item shall be removed from the player inventory array, and added to the area inventory array. Returns the player to the inventory screen, which no longer displays the item that was dropped.</t>
+  </si>
+  <si>
+    <t>Type q to return to the game menu</t>
+  </si>
+  <si>
+    <t>Displays game menu</t>
+  </si>
+  <si>
+    <t>Type P</t>
+  </si>
+  <si>
+    <t>Open the Inventory file</t>
+  </si>
+  <si>
+    <t>Typing P prints the player inventory (from the last screen) to a file on the computer. A suitable filepath must be typed in, or the file will be saved to the directory that the executable was run from.
+ Enter a filepath where the report will output: 
+F:\tcchr\Desktop\inventory.txt
+Report successfully saved to F:\tcchr\Desktop\inventory.txt</t>
+  </si>
+  <si>
+    <t>Open the inventory file, should display the same items from the Inventory Screen and have no glitches
+     Inventory Report
+Item Name            Cost
+-------------------------
+Shelter                20
+Shotgun                 9
+Granola Bar             5
+Scrap Iron              0
+Resource              200</t>
+  </si>
+  <si>
+    <t>In the program, type PI</t>
+  </si>
+  <si>
+    <t>Does the same thing as the last menu, only it prints the items on the ground to a file.</t>
+  </si>
+  <si>
+    <t>Open the saved inventory file</t>
+  </si>
+  <si>
+    <t>Check that the items match what the game displays and that it prints neatly</t>
+  </si>
+  <si>
+    <t>Type q to return to the main menu</t>
+  </si>
+  <si>
+    <t>Displays the Main Menu</t>
+  </si>
+  <si>
+    <t>Type S to save the game</t>
+  </si>
+  <si>
+    <t>Displays the save text, asks the user to supply a filepath to save the game to.
+Should display a confirmation that the game saves succesfully and the path it was saved to</t>
+  </si>
+  <si>
+    <t>The program fails this one. I didn't have time to troubleshoot the java.io.PrintWriter error that I was getting when I tried to save all of the active objects to the save file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type L </t>
+  </si>
+  <si>
+    <t>Displays the load game interface, asks for a path to a save game file. Loads all of the objects from the file to start the player from where they last were.  Displays the welcome back text "Welcome Back, please don't die!" Displays the Game menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type q </t>
+  </si>
+  <si>
+    <t>Quit back to the main menu, display main menu</t>
+  </si>
+  <si>
+    <t>Type H</t>
+  </si>
+  <si>
+    <t>Displays the help menu
+****************************************
+                 Help Menu              
+P : How to Play
+W : How to Win
+Q : Quit
+****************************************</t>
+  </si>
+  <si>
+    <t>Type p</t>
+  </si>
+  <si>
+    <t>Displays the "How to Play" text</t>
+  </si>
+  <si>
+    <t>Type q</t>
+  </si>
+  <si>
+    <t>Returns the user to the Help menu</t>
+  </si>
+  <si>
+    <t>Type W</t>
+  </si>
+  <si>
+    <t>Displays the "How to Win" text, returns the player to the help menu
+Fill your pack with the nessecary supplies to make the journey before you get eaten!</t>
+  </si>
+  <si>
+    <t>Returns the user to the Main Menu</t>
+  </si>
+  <si>
+    <t>Type G</t>
+  </si>
+  <si>
+    <t>Displays the Game Menu, this is used if the player has resumed a game, and does not wish to start a new game. Will display an error "No game started" if the initialization variables are not set.</t>
+  </si>
+  <si>
+    <t>Type q to quite</t>
+  </si>
+  <si>
+    <t>Quits the game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +472,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,18 +515,18 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,29 +842,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="84.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -522,85 +881,474 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>21</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>23</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>24</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>29</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>31</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>33</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>35</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>36</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>37</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>38</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>39</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -614,5 +1362,6 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>